<commit_message>
performed two tailed t-tests on adaboost classifiers vs all the other classifiers on gym movements dataset
</commit_message>
<xml_diff>
--- a/Evaluation/rocket_two_tailed_t-tests.xlsx
+++ b/Evaluation/rocket_two_tailed_t-tests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redma\Documents\GitHub\ExerciseClassification\t-test accuracy results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redma\Documents\GitHub\ExerciseClassification\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B0B064-D84B-46BC-B2E8-34709CFE5C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E2D013-F384-444B-8173-BB54286E086F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rocket vs AdaBoost" sheetId="2" r:id="rId1"/>
@@ -124,64 +124,64 @@
     <t>Time Series Forest</t>
   </si>
   <si>
-    <t>H0: there is no difference in mean accuracry between Rocket and AdaBoost on gym movements</t>
-  </si>
-  <si>
-    <t>H1: there is a difference in mean accuracry between Rocket and AdaBoost on gym movements</t>
-  </si>
-  <si>
-    <t>H0: there is no difference in mean accuracry between Rocket and Boss Ensemble on gym movements</t>
-  </si>
-  <si>
-    <t>H1: there is a difference in mean accuracry between Rocket and Boss Ensemble on gym movements</t>
-  </si>
-  <si>
     <t xml:space="preserve">Based off the evidence of this test we cannot reject the null hypothesis </t>
   </si>
   <si>
     <t xml:space="preserve">Based off the evidence of this test we can reject the null hypothesis </t>
   </si>
   <si>
-    <t>H0: there is no difference in mean accuracry between Rocket and Decision Tree on gym movements</t>
-  </si>
-  <si>
-    <t>H1: there is a difference in mean accuracry between Rocket and Decision Tree on gym movements</t>
-  </si>
-  <si>
-    <t>H0: there is no difference in mean accuracry between Rocket and kNN-ED on gym movements</t>
-  </si>
-  <si>
-    <t>H1: there is a difference in mean accuracry between Rocket and kNN-ED on gym movements</t>
-  </si>
-  <si>
-    <t>H0: there is no difference in mean accuracry between Rocket and kNN-DTW on gym movements</t>
-  </si>
-  <si>
-    <t>H1: there is a difference in mean accuracry between Rocket and kNN-DTW on gym movements</t>
-  </si>
-  <si>
-    <t>H0: there is no difference in mean accuracry between Rocket and MLP on gym movements</t>
-  </si>
-  <si>
-    <t>H1: there is a difference in mean accuracry between Rocket and MLP on gym movements</t>
-  </si>
-  <si>
-    <t>H0: there is no difference in mean accuracry between Rocket and Naïve Bayes on gym movements</t>
-  </si>
-  <si>
-    <t>H1: there is a difference in mean accuracry between Rocket and Naïve Bayes on gym movements</t>
-  </si>
-  <si>
-    <t>H0: there is no difference in mean accuracry between Rocket and Random Forest on gym movements</t>
-  </si>
-  <si>
-    <t>H1: there is a difference in mean accuracry between Rocket and Random Forest on gym movements</t>
-  </si>
-  <si>
-    <t>H0: there is no difference in mean accuracry between Rocket and Time Series Forest on gym movements</t>
-  </si>
-  <si>
-    <t>H1: there is a difference in mean accuracry between Rocket and Time Series Forest on gym movements</t>
+    <t>H0: there is no difference in mean accuracy between Rocket and Time Series Forest on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracy between Rocket and Time Series Forest on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracy between Rocket and Random Forest on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracy between Rocket and Random Forest on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracy between Rocket and Naïve Bayes on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracy between Rocket and Naïve Bayes on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracy between Rocket and MLP on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracy between Rocket and MLP on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracy between Rocket and kNN-DTW on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracy between Rocket and kNN-DTW on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracy between Rocket and kNN-ED on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracy between Rocket and kNN-ED on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracy between Rocket and Decision Tree on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracy between Rocket and Decision Tree on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracy between Rocket and Boss Ensemble on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracy between Rocket and Boss Ensemble on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracy between Rocket and AdaBoost on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracy between Rocket and AdaBoost on gym movements</t>
   </si>
 </sst>
 </file>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181FC21C-74BD-47D5-A002-640CBAB53DA8}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="A17:H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -908,7 +908,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -920,7 +920,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -932,7 +932,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -956,7 +956,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="A17:H20"/>
+      <selection activeCell="A18" sqref="A18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -1300,7 +1300,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="A17:H20"/>
+      <selection activeCell="A18" sqref="A18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -1621,7 +1621,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -1644,7 +1644,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="A17:H20"/>
+      <selection activeCell="A18" sqref="A18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -1991,7 +1991,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:H20"/>
+      <selection activeCell="A18" sqref="A18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -2354,7 +2354,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="A17:H20"/>
+      <selection activeCell="A18" sqref="A18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2661,7 +2661,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -2673,7 +2673,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -2685,7 +2685,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -2708,7 +2708,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="A17:H20"/>
+      <selection activeCell="A18" sqref="A18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -3018,7 +3018,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -3053,7 +3053,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="A17:H20"/>
+      <selection activeCell="A18" sqref="A18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3350,7 +3350,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -3362,7 +3362,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -3374,7 +3374,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -3396,8 +3396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F920CD64-38D7-4C34-AE1D-7F46FDF00FF8}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3695,7 +3695,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -3707,7 +3707,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -3719,7 +3719,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>

</xml_diff>